<commit_message>
Updated llm cost calculations to make the formula easier to read and include the RAG query and Guardrails costs.
</commit_message>
<xml_diff>
--- a/Research/llm-cost-calculations.xlsx
+++ b/Research/llm-cost-calculations.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://libertymutualeur-my.sharepoint.com/personal/karl_kyck_liberty-it_co_uk/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="8_{C90E617D-097C-0549-AF67-C02E81F1E5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98A34D7D-A520-F44F-8EA3-5C5F4DD88FC1}"/>
+  <xr:revisionPtr revIDLastSave="281" documentId="8_{C90E617D-097C-0549-AF67-C02E81F1E5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B493EBB3-2842-714E-8312-084897098E91}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="21260" xr2:uid="{DC820DE9-C478-F446-8EEE-5581CF15CA61}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="27180" xr2:uid="{DC820DE9-C478-F446-8EEE-5581CF15CA61}"/>
   </bookViews>
   <sheets>
-    <sheet name="Costings" sheetId="1" r:id="rId1"/>
+    <sheet name="Costings (2)" sheetId="6" r:id="rId1"/>
     <sheet name="Assumptions" sheetId="4" r:id="rId2"/>
     <sheet name="Models" sheetId="2" r:id="rId3"/>
     <sheet name="Tools" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -75,12 +75,6 @@
     <t>PP 1000 input tokens</t>
   </si>
   <si>
-    <t>Guard rails</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Knowledge bases per query </t>
-  </si>
-  <si>
     <t>Test 1 tokens</t>
   </si>
   <si>
@@ -112,6 +106,12 @@
   </si>
   <si>
     <t>Test 2 num personas</t>
+  </si>
+  <si>
+    <t>Guard rails per token</t>
+  </si>
+  <si>
+    <t>Knowledge bases per query</t>
   </si>
 </sst>
 </file>
@@ -497,48 +497,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236062E0-2C2E-D74B-BFB6-0C0ACE7AFDC1}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EEE00A3-97EF-EE4A-A507-5876E221F88A}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="A1:D2"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" cm="1">
-        <f t="array" aca="1" ref="C2" ca="1">((INDIRECT("Assumptions!B"&amp;MATCH(A2, Assumptions!A2:A10, 0)+1)/1000)*(INDIRECT("Models!B"&amp;MATCH(B2, Models!A2:A10, 0)+1))+(INDIRECT("Models!C"&amp;MATCH(B2, Models!A2:A10, 0)+1)/1000))*(INDIRECT("Assumptions!C"&amp;MATCH(A2, Assumptions!A2:A10, 0)+1))</f>
-        <v>0.16201080000000001</v>
-      </c>
-      <c r="D2" cm="1">
-        <f t="array" aca="1" ref="D2" ca="1">(((INDIRECT("Assumptions!D"&amp;MATCH(A2, Assumptions!A2:A10, 0)+1)/1000)*(INDIRECT("Models!B"&amp;MATCH(B2, Models!A2:A10, 0)+1))+(INDIRECT("Models!C"&amp;MATCH(B2, Models!A2:A10, 0)+1)/1000))*(INDIRECT("Assumptions!E"&amp;MATCH(A2, Assumptions!A2:A10, 0)+1)))+Tools!A2+Tools!B2</f>
-        <v>1.3130054000000002</v>
+      <c r="C2">
+        <f ca="1">(F2*(K2/1000)*G2)+(N2*G2)+(O2*F2)</f>
+        <v>0.28200000000000003</v>
+      </c>
+      <c r="D2">
+        <f ca="1">((H2*(K2/1000))*I2)+(N2*I2)+(O2*H2)</f>
+        <v>1.155</v>
+      </c>
+      <c r="F2" cm="1">
+        <f t="array" aca="1" ref="F2" ca="1">(INDIRECT("Assumptions!B"&amp;MATCH(A2,Assumptions!A2:A10,0)+1))</f>
+        <v>15000</v>
+      </c>
+      <c r="G2" cm="1">
+        <f t="array" aca="1" ref="G2" ca="1">(INDIRECT("Assumptions!C"&amp;MATCH(A2,Assumptions!A2:A10,0)+1))</f>
+        <v>30</v>
+      </c>
+      <c r="H2" cm="1">
+        <f t="array" aca="1" ref="H2" ca="1">(INDIRECT("Assumptions!D"&amp;MATCH(A2,Assumptions!A2:A10,0)+1))</f>
+        <v>150000</v>
+      </c>
+      <c r="I2" cm="1">
+        <f t="array" aca="1" ref="I2" ca="1">(INDIRECT("Assumptions!E"&amp;MATCH(A2,Assumptions!A2:A10,0)+1))</f>
+        <v>15</v>
+      </c>
+      <c r="K2" cm="1">
+        <f t="array" aca="1" ref="K2" ca="1">INDIRECT("Models!B"&amp;MATCH(B2,Models!A2:A10,0)+1)</f>
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="L2" cm="1">
+        <f t="array" aca="1" ref="L2" ca="1">INDIRECT("Models!C"&amp;MATCH(B2,Models!A2:A10,0)+1)</f>
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="N2">
+        <f>Tools!A2</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="O2">
+        <f>Tools!B2</f>
+        <v>1.9999999999999999E-6</v>
       </c>
     </row>
   </sheetData>
@@ -546,17 +611,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{612DDE2B-8C10-CC41-A029-6EAD50A7234F}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B06F82F4-4313-E14D-80C0-471971B1E59C}">
+          <x14:formula1>
+            <xm:f>Assumptions!$A$2:$A$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{90B27DD7-793F-DA4C-BA3C-897C9E862B7C}">
           <x14:formula1>
             <xm:f>Models!$A$2:$A$24</xm:f>
           </x14:formula1>
           <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E150FCD5-C3A6-354D-9D86-74F3A82605C1}">
-          <x14:formula1>
-            <xm:f>Assumptions!$A$2:$A$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -570,7 +635,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E4"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,24 +649,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>5000</v>
@@ -618,7 +683,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>10000</v>
@@ -635,7 +700,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>15000</v>
@@ -661,8 +726,8 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C3"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,7 +761,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2">
         <v>1.5E-3</v>
@@ -717,7 +782,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,10 +792,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -738,7 +803,8 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <f>(0.5/1000000)*4</f>
+        <v>1.9999999999999999E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>